<commit_message>
assortment , pln summary
</commit_message>
<xml_diff>
--- a/Projects/GSKSG_SAND2/Data/gsk_set_up.xlsx
+++ b/Projects/GSKSG_SAND2/Data/gsk_set_up.xlsx
@@ -14,7 +14,7 @@
     <externalReference r:id="rId3"/>
   </externalReferences>
   <definedNames>
-    <definedName function="false" hidden="false" name="Validation_List" vbProcedure="false">[1]Set_up!$A$90:$A$124</definedName>
+    <definedName function="false" hidden="false" name="Validation_List" vbProcedure="false">[2]Set_up!$A$90:$A$124</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">'Functional KPIs'!$A$1:$J$4</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="19">
   <si>
     <t xml:space="preserve">KPI Type</t>
   </si>
@@ -81,6 +81,9 @@
   </si>
   <si>
     <t xml:space="preserve">Availability</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Orange Score</t>
   </si>
 </sst>
 </file>
@@ -90,7 +93,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="7">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -127,6 +130,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="3">
@@ -191,7 +200,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -226,6 +235,10 @@
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -300,7 +313,7 @@
 </styleSheet>
 </file>
 
-<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/externalLinks/externalLink2.xml><?xml version="1.0" encoding="utf-8"?>
 <externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
 </externalLink>
@@ -311,28 +324,28 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="1:4"/>
+  <dimension ref="1:5"/>
   <sheetViews>
     <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="70" zoomScaleNormal="70" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="4" ySplit="1" topLeftCell="E2" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="E1" activeCellId="0" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="L1" activeCellId="0" sqref="L1"/>
+      <selection pane="bottomRight" activeCell="J5" activeCellId="0" sqref="J5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="20.246963562753"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="20.3522267206478"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="1" width="10.3886639676113"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="27.6356275303644"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="15.7449392712551"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="15.5303643724696"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="27.8502024291498"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="15.8542510121457"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="15.6396761133603"/>
     <col collapsed="false" hidden="false" max="6" min="6" style="1" width="13.9271255060729"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="20.3522267206478"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="20.4615384615385"/>
     <col collapsed="false" hidden="false" max="9" min="8" style="1" width="11.0323886639676"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="20.5668016194332"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="1" width="27.2064777327935"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="20.6720647773279"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="1" width="27.4210526315789"/>
     <col collapsed="false" hidden="false" max="1014" min="12" style="1" width="8.78542510121457"/>
     <col collapsed="false" hidden="false" max="1025" min="1015" style="0" width="8.78542510121457"/>
   </cols>
@@ -459,6 +472,14 @@
       <c r="F4" s="5"/>
       <c r="G4" s="8"/>
     </row>
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="J5" s="9" t="s">
+        <v>15</v>
+      </c>
+    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>

</xml_diff>

<commit_message>
adding filtering to scif
</commit_message>
<xml_diff>
--- a/Projects/GSKSG_SAND2/Data/gsk_set_up.xlsx
+++ b/Projects/GSKSG_SAND2/Data/gsk_set_up.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="22">
   <si>
     <t xml:space="preserve">KPI Type</t>
   </si>
@@ -84,6 +84,15 @@
   </si>
   <si>
     <t xml:space="preserve">Availability</t>
+  </si>
+  <si>
+    <t xml:space="preserve">planogram</t>
+  </si>
+  <si>
+    <t xml:space="preserve">secondary_display</t>
+  </si>
+  <si>
+    <t xml:space="preserve">promo</t>
   </si>
 </sst>
 </file>
@@ -136,6 +145,7 @@
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <charset val="177"/>
     </font>
   </fonts>
   <fills count="3">
@@ -238,11 +248,11 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -328,28 +338,28 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="1:4"/>
+  <dimension ref="1:7"/>
   <sheetViews>
     <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="70" zoomScaleNormal="70" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="4" ySplit="1" topLeftCell="E2" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="E1" activeCellId="0" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="O17" activeCellId="0" sqref="O17"/>
+      <selection pane="bottomRight" activeCell="C2" activeCellId="0" sqref="C2:C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="20.3522267206478"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="20.6720647773279"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="1" width="10.3886639676113"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="27.8502024291498"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="15.8542510121457"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="15.6396761133603"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="28.4939271255061"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="16.1740890688259"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="15.9595141700405"/>
     <col collapsed="false" hidden="false" max="6" min="6" style="1" width="13.9271255060729"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="20.4615384615385"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="20.7813765182186"/>
     <col collapsed="false" hidden="false" max="9" min="8" style="1" width="11.0323886639676"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="20.6720647773279"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="1" width="27.4210526315789"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="20.995951417004"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="1" width="28.0647773279352"/>
     <col collapsed="false" hidden="false" max="1014" min="12" style="1" width="8.78542510121457"/>
     <col collapsed="false" hidden="false" max="1025" min="1015" style="0" width="8.78542510121457"/>
   </cols>
@@ -407,7 +417,7 @@
         <v>12</v>
       </c>
       <c r="B2" s="6"/>
-      <c r="C2" s="6"/>
+      <c r="C2" s="7"/>
       <c r="D2" s="7" t="s">
         <v>13</v>
       </c>
@@ -445,7 +455,7 @@
         <v>17</v>
       </c>
       <c r="B3" s="6"/>
-      <c r="C3" s="6"/>
+      <c r="C3" s="7"/>
       <c r="D3" s="7" t="s">
         <v>14</v>
       </c>
@@ -464,7 +474,7 @@
         <v>15</v>
       </c>
       <c r="K3" s="7"/>
-      <c r="L3" s="9" t="s">
+      <c r="L3" s="7" t="s">
         <v>16</v>
       </c>
     </row>
@@ -479,8 +489,44 @@
       </c>
       <c r="F4" s="5"/>
       <c r="G4" s="8"/>
-      <c r="L4" s="10" t="s">
+      <c r="L4" s="5" t="s">
         <v>16</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C5" s="9"/>
+      <c r="D5" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="L5" s="7" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C6" s="9"/>
+      <c r="D6" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="L6" s="7" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C7" s="10"/>
+      <c r="D7" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="L7" s="5" t="s">
+        <v>14</v>
       </c>
     </row>
   </sheetData>

</xml_diff>